<commit_message>
Examples added for Aspose.Cells for Java 18.10
</commit_message>
<xml_diff>
--- a/Examples/src/resources/02_OutputDirectory/outSourseSampleCountryNames.xlsx
+++ b/Examples/src/resources/02_OutputDirectory/outSourseSampleCountryNames.xlsx
@@ -564,22 +564,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15">
+    <row r="2" spans="1:1" ht="15" hidden="1">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15">
+    <row r="3" spans="1:1" ht="15" hidden="1">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15">
+    <row r="4" spans="1:1" ht="15" hidden="1">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15">
+    <row r="5" spans="1:1" ht="15" hidden="1">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -609,12 +609,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15" hidden="1">
+    <row r="11" spans="1:1" ht="15">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="15" hidden="1">
+    <row r="12" spans="1:1" ht="15">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -634,7 +634,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="15" hidden="1">
+    <row r="16" spans="1:1" ht="15">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -653,7 +653,7 @@
   <autoFilter ref="A1:A18">
     <filterColumn colId="0">
       <customFilters>
-        <customFilter val="*Ba*"/>
+        <customFilter val="*ia"/>
       </customFilters>
     </filterColumn>
   </autoFilter>

</xml_diff>